<commit_message>
bumped into a problem
reactive parameters values not updating w/o bringing up the input window
</commit_message>
<xml_diff>
--- a/v13_newUI/www/data/parameters.xlsx
+++ b/v13_newUI/www/data/parameters.xlsx
@@ -1215,8 +1215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="G16" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -1794,16 +1794,19 @@
         <v>101</v>
       </c>
       <c r="G17" s="2">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>97</v>
       </c>
       <c r="I17" s="2">
+        <v>0</v>
+      </c>
+      <c r="J17" s="2">
+        <v>80</v>
+      </c>
+      <c r="K17" s="2">
         <v>1</v>
-      </c>
-      <c r="J17" s="2">
-        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:11">

</xml_diff>

<commit_message>
woking version except for par update
</commit_message>
<xml_diff>
--- a/v13_newUI/www/data/parameters.xlsx
+++ b/v13_newUI/www/data/parameters.xlsx
@@ -1215,11 +1215,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G16" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="16.8" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="11.296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.69921875" customWidth="1"/>
@@ -1227,12 +1227,14 @@
     <col min="4" max="4" width="21.5" customWidth="1"/>
     <col min="5" max="5" width="60.19921875" customWidth="1"/>
     <col min="6" max="6" width="91.296875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="63.19921875" customWidth="1"/>
+    <col min="7" max="7" width="15.3984375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.296875" customWidth="1"/>
-    <col min="9" max="9" width="49.19921875" customWidth="1"/>
+    <col min="9" max="9" width="6.59765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.8984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" ht="16.8" customHeight="1">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1267,7 +1269,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" ht="16.8" customHeight="1">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1290,7 +1292,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" ht="16.8" customHeight="1">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1319,7 +1321,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="140.4">
+    <row r="4" spans="1:11" ht="16.8" customHeight="1">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1354,7 +1356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="31.2">
+    <row r="5" spans="1:11" ht="16.8" customHeight="1">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1389,7 +1391,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="31.2">
+    <row r="6" spans="1:11" ht="16.8" customHeight="1">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1424,7 +1426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="2" customFormat="1" ht="46.8">
+    <row r="7" spans="1:11" s="2" customFormat="1" ht="16.8" customHeight="1">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1459,7 +1461,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="2" customFormat="1" ht="31.2">
+    <row r="8" spans="1:11" s="2" customFormat="1" ht="16.8" customHeight="1">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -1494,7 +1496,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="2" customFormat="1" ht="78">
+    <row r="9" spans="1:11" s="2" customFormat="1" ht="16.8" customHeight="1">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1529,7 +1531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="2" customFormat="1" ht="46.8">
+    <row r="10" spans="1:11" s="2" customFormat="1" ht="16.8" customHeight="1">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1564,7 +1566,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="2" customFormat="1" ht="78">
+    <row r="11" spans="1:11" s="2" customFormat="1" ht="16.8" customHeight="1">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1599,7 +1601,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="2" customFormat="1" ht="78">
+    <row r="12" spans="1:11" s="2" customFormat="1" ht="16.8" customHeight="1">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1634,7 +1636,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="2" customFormat="1" ht="93.6">
+    <row r="13" spans="1:11" s="2" customFormat="1" ht="16.8" customHeight="1">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1669,7 +1671,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="2" customFormat="1" ht="46.8">
+    <row r="14" spans="1:11" s="2" customFormat="1" ht="16.8" customHeight="1">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1704,7 +1706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="2" customFormat="1" ht="171.6">
+    <row r="15" spans="1:11" s="2" customFormat="1" ht="16.8" customHeight="1">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1739,7 +1741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="2" customFormat="1" ht="171.6">
+    <row r="16" spans="1:11" s="2" customFormat="1" ht="16.8" customHeight="1">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1774,7 +1776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="2" customFormat="1">
+    <row r="17" spans="1:11" s="2" customFormat="1" ht="16.8" customHeight="1">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -1809,7 +1811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" ht="16.8" customHeight="1">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -1835,7 +1837,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" ht="16.8" customHeight="1">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -1861,7 +1863,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" ht="16.8" customHeight="1">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -1896,7 +1898,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" ht="16.8" customHeight="1">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1931,7 +1933,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" ht="16.8" customHeight="1">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -1957,7 +1959,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" ht="16.8" customHeight="1">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -1992,7 +1994,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" ht="16.8" customHeight="1">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -2012,7 +2014,7 @@
         <v>22</v>
       </c>
       <c r="G24">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="H24" t="s">
         <v>97</v>
@@ -2027,7 +2029,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" ht="16.8" customHeight="1">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -2053,7 +2055,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" ht="16.8" customHeight="1">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -2088,7 +2090,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" ht="16.8" customHeight="1">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -2123,7 +2125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" ht="16.8" customHeight="1">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -2158,7 +2160,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" ht="16.8" customHeight="1">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -2193,7 +2195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" ht="16.8" customHeight="1">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -2219,7 +2221,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" ht="16.8" customHeight="1">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -2239,7 +2241,7 @@
         <v>53</v>
       </c>
       <c r="G31">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="H31" t="s">
         <v>97</v>
@@ -2248,13 +2250,13 @@
         <v>5</v>
       </c>
       <c r="J31">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="K31">
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" ht="16.8" customHeight="1">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -2289,7 +2291,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" ht="16.8" customHeight="1">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -2324,7 +2326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" ht="16.8" customHeight="1">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -2359,7 +2361,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" ht="16.8" customHeight="1">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -2394,7 +2396,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" ht="16.8" customHeight="1">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -2429,7 +2431,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" ht="16.8" customHeight="1">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -2464,7 +2466,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" ht="16.8" customHeight="1">
       <c r="A38" t="s">
         <v>10</v>
       </c>
@@ -2487,7 +2489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" ht="16.8" customHeight="1">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -2522,7 +2524,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:11" ht="16.8" customHeight="1">
       <c r="A40" t="s">
         <v>10</v>
       </c>
@@ -2557,7 +2559,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:11" ht="16.8" customHeight="1">
       <c r="A41" t="s">
         <v>10</v>
       </c>
@@ -2580,7 +2582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:11" ht="16.8" customHeight="1">
       <c r="A42" t="s">
         <v>10</v>
       </c>
@@ -2615,7 +2617,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" ht="16.8" customHeight="1">
       <c r="A43" t="s">
         <v>10</v>
       </c>
@@ -2650,7 +2652,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:11" ht="16.8" customHeight="1">
       <c r="A44" t="s">
         <v>10</v>
       </c>
@@ -2685,7 +2687,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:11" ht="16.8" customHeight="1">
       <c r="A45" t="s">
         <v>10</v>
       </c>
@@ -2720,7 +2722,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:11" ht="16.8" customHeight="1">
       <c r="A46" t="s">
         <v>10</v>
       </c>
@@ -2755,7 +2757,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:11" ht="16.8" customHeight="1">
       <c r="A47" t="s">
         <v>10</v>
       </c>
@@ -2778,7 +2780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:11" ht="16.8" customHeight="1">
       <c r="A48" t="s">
         <v>10</v>
       </c>
@@ -2813,7 +2815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:11" ht="16.8" customHeight="1">
       <c r="A49" t="s">
         <v>10</v>
       </c>
@@ -2848,7 +2850,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="50" spans="1:11">
+    <row r="50" spans="1:11" ht="16.8" customHeight="1">
       <c r="A50" t="s">
         <v>10</v>
       </c>
@@ -2883,7 +2885,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:11" ht="16.8" customHeight="1">
       <c r="A51" t="s">
         <v>10</v>
       </c>
@@ -2918,7 +2920,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:11" ht="16.8" customHeight="1">
       <c r="A52" t="s">
         <v>10</v>
       </c>
@@ -2953,7 +2955,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="31.2">
+    <row r="53" spans="1:11" ht="16.8" customHeight="1">
       <c r="A53" t="s">
         <v>10</v>
       </c>
@@ -2988,7 +2990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="31.2">
+    <row r="54" spans="1:11" ht="16.8" customHeight="1">
       <c r="A54" t="s">
         <v>10</v>
       </c>
@@ -3023,7 +3025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="31.2">
+    <row r="55" spans="1:11" ht="16.8" customHeight="1">
       <c r="A55" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
with Olivier's changes to UI. fully running
</commit_message>
<xml_diff>
--- a/v13_newUI/www/data/parameters.xlsx
+++ b/v13_newUI/www/data/parameters.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\IBM project_Sai\RAI model\v13_newUI\www\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27420" windowHeight="17544" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27420" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="inputs" sheetId="1" r:id="rId1"/>
@@ -510,12 +505,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1215,26 +1211,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="16.8" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.69921875" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
     <col min="3" max="3" width="21.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.5" customWidth="1"/>
-    <col min="5" max="5" width="60.19921875" customWidth="1"/>
-    <col min="6" max="6" width="91.296875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="15.3984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.296875" customWidth="1"/>
-    <col min="9" max="9" width="6.59765625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.8984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="60.1640625" customWidth="1"/>
+    <col min="6" max="6" width="91.33203125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.8" customHeight="1">
+    <row r="1" spans="1:11" ht="16.75" customHeight="1">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1269,7 +1265,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="16.8" customHeight="1">
+    <row r="2" spans="1:11" ht="16.75" customHeight="1">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1292,7 +1288,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="16.8" customHeight="1">
+    <row r="3" spans="1:11" ht="16.75" customHeight="1">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1321,7 +1317,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="16.8" customHeight="1">
+    <row r="4" spans="1:11" ht="16.75" customHeight="1">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1356,7 +1352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="16.8" customHeight="1">
+    <row r="5" spans="1:11" ht="16.75" customHeight="1">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1391,7 +1387,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="16.8" customHeight="1">
+    <row r="6" spans="1:11" ht="16.75" customHeight="1">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1426,7 +1422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="2" customFormat="1" ht="16.8" customHeight="1">
+    <row r="7" spans="1:11" s="2" customFormat="1" ht="16.75" customHeight="1">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1461,7 +1457,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="2" customFormat="1" ht="16.8" customHeight="1">
+    <row r="8" spans="1:11" s="2" customFormat="1" ht="16.75" customHeight="1">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -1496,7 +1492,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="2" customFormat="1" ht="16.8" customHeight="1">
+    <row r="9" spans="1:11" s="2" customFormat="1" ht="16.75" customHeight="1">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1531,7 +1527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="2" customFormat="1" ht="16.8" customHeight="1">
+    <row r="10" spans="1:11" s="2" customFormat="1" ht="16.75" customHeight="1">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1566,7 +1562,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="2" customFormat="1" ht="16.8" customHeight="1">
+    <row r="11" spans="1:11" s="2" customFormat="1" ht="16.75" customHeight="1">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1601,7 +1597,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="2" customFormat="1" ht="16.8" customHeight="1">
+    <row r="12" spans="1:11" s="2" customFormat="1" ht="16.75" customHeight="1">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1636,7 +1632,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="2" customFormat="1" ht="16.8" customHeight="1">
+    <row r="13" spans="1:11" s="2" customFormat="1" ht="16.75" customHeight="1">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1671,7 +1667,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="2" customFormat="1" ht="16.8" customHeight="1">
+    <row r="14" spans="1:11" s="2" customFormat="1" ht="16.75" customHeight="1">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1706,7 +1702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="2" customFormat="1" ht="16.8" customHeight="1">
+    <row r="15" spans="1:11" s="2" customFormat="1" ht="16.75" customHeight="1">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1741,7 +1737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="2" customFormat="1" ht="16.8" customHeight="1">
+    <row r="16" spans="1:11" s="2" customFormat="1" ht="16.75" customHeight="1">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1776,7 +1772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="2" customFormat="1" ht="16.8" customHeight="1">
+    <row r="17" spans="1:11" s="2" customFormat="1" ht="16.75" customHeight="1">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -1811,7 +1807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="16.8" customHeight="1">
+    <row r="18" spans="1:11" ht="16.75" customHeight="1">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -1837,7 +1833,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="16.8" customHeight="1">
+    <row r="19" spans="1:11" ht="16.75" customHeight="1">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -1863,7 +1859,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="16.8" customHeight="1">
+    <row r="20" spans="1:11" ht="16.75" customHeight="1">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -1898,7 +1894,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="16.8" customHeight="1">
+    <row r="21" spans="1:11" ht="16.75" customHeight="1">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1933,7 +1929,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="16.8" customHeight="1">
+    <row r="22" spans="1:11" ht="16.75" customHeight="1">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -1959,7 +1955,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="16.8" customHeight="1">
+    <row r="23" spans="1:11" ht="16.75" customHeight="1">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -1994,7 +1990,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="16.8" customHeight="1">
+    <row r="24" spans="1:11" ht="16.75" customHeight="1">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -2029,7 +2025,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="16.8" customHeight="1">
+    <row r="25" spans="1:11" ht="16.75" customHeight="1">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -2055,7 +2051,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="16.8" customHeight="1">
+    <row r="26" spans="1:11" ht="16.75" customHeight="1">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -2090,7 +2086,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="16.8" customHeight="1">
+    <row r="27" spans="1:11" ht="16.75" customHeight="1">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -2125,7 +2121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="16.8" customHeight="1">
+    <row r="28" spans="1:11" ht="16.75" customHeight="1">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -2160,7 +2156,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="16.8" customHeight="1">
+    <row r="29" spans="1:11" ht="16.75" customHeight="1">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -2195,7 +2191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="16.8" customHeight="1">
+    <row r="30" spans="1:11" ht="16.75" customHeight="1">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -2221,7 +2217,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="16.8" customHeight="1">
+    <row r="31" spans="1:11" ht="16.75" customHeight="1">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -2256,7 +2252,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="16.8" customHeight="1">
+    <row r="32" spans="1:11" ht="16.75" customHeight="1">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -2291,7 +2287,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="16.8" customHeight="1">
+    <row r="33" spans="1:11" ht="16.75" customHeight="1">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -2326,7 +2322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="16.8" customHeight="1">
+    <row r="34" spans="1:11" ht="16.75" customHeight="1">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -2361,7 +2357,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="16.8" customHeight="1">
+    <row r="35" spans="1:11" ht="16.75" customHeight="1">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -2396,7 +2392,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="16.8" customHeight="1">
+    <row r="36" spans="1:11" ht="16.75" customHeight="1">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -2431,7 +2427,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="16.8" customHeight="1">
+    <row r="37" spans="1:11" ht="16.75" customHeight="1">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -2466,7 +2462,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="16.8" customHeight="1">
+    <row r="38" spans="1:11" ht="16.75" customHeight="1">
       <c r="A38" t="s">
         <v>10</v>
       </c>
@@ -2489,7 +2485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="16.8" customHeight="1">
+    <row r="39" spans="1:11" ht="16.75" customHeight="1">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -2524,7 +2520,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="16.8" customHeight="1">
+    <row r="40" spans="1:11" ht="16.75" customHeight="1">
       <c r="A40" t="s">
         <v>10</v>
       </c>
@@ -2559,7 +2555,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="16.8" customHeight="1">
+    <row r="41" spans="1:11" ht="16.75" customHeight="1">
       <c r="A41" t="s">
         <v>10</v>
       </c>
@@ -2582,7 +2578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="16.8" customHeight="1">
+    <row r="42" spans="1:11" ht="16.75" customHeight="1">
       <c r="A42" t="s">
         <v>10</v>
       </c>
@@ -2617,7 +2613,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="16.8" customHeight="1">
+    <row r="43" spans="1:11" ht="16.75" customHeight="1">
       <c r="A43" t="s">
         <v>10</v>
       </c>
@@ -2652,7 +2648,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="16.8" customHeight="1">
+    <row r="44" spans="1:11" ht="16.75" customHeight="1">
       <c r="A44" t="s">
         <v>10</v>
       </c>
@@ -2687,7 +2683,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="16.8" customHeight="1">
+    <row r="45" spans="1:11" ht="16.75" customHeight="1">
       <c r="A45" t="s">
         <v>10</v>
       </c>
@@ -2722,7 +2718,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="16.8" customHeight="1">
+    <row r="46" spans="1:11" ht="16.75" customHeight="1">
       <c r="A46" t="s">
         <v>10</v>
       </c>
@@ -2757,7 +2753,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="16.8" customHeight="1">
+    <row r="47" spans="1:11" ht="16.75" customHeight="1">
       <c r="A47" t="s">
         <v>10</v>
       </c>
@@ -2780,7 +2776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="16.8" customHeight="1">
+    <row r="48" spans="1:11" ht="16.75" customHeight="1">
       <c r="A48" t="s">
         <v>10</v>
       </c>
@@ -2815,7 +2811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="16.8" customHeight="1">
+    <row r="49" spans="1:11" ht="16.75" customHeight="1">
       <c r="A49" t="s">
         <v>10</v>
       </c>
@@ -2850,7 +2846,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="16.8" customHeight="1">
+    <row r="50" spans="1:11" ht="16.75" customHeight="1">
       <c r="A50" t="s">
         <v>10</v>
       </c>
@@ -2885,7 +2881,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="16.8" customHeight="1">
+    <row r="51" spans="1:11" ht="16.75" customHeight="1">
       <c r="A51" t="s">
         <v>10</v>
       </c>
@@ -2920,7 +2916,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="16.8" customHeight="1">
+    <row r="52" spans="1:11" ht="16.75" customHeight="1">
       <c r="A52" t="s">
         <v>10</v>
       </c>
@@ -2955,7 +2951,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="16.8" customHeight="1">
+    <row r="53" spans="1:11" ht="16.75" customHeight="1">
       <c r="A53" t="s">
         <v>10</v>
       </c>
@@ -2990,7 +2986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="16.8" customHeight="1">
+    <row r="54" spans="1:11" ht="16.75" customHeight="1">
       <c r="A54" t="s">
         <v>10</v>
       </c>
@@ -3025,7 +3021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="16.8" customHeight="1">
+    <row r="55" spans="1:11" ht="16.75" customHeight="1">
       <c r="A55" t="s">
         <v>10</v>
       </c>

</xml_diff>